<commit_message>
figure and supp file arrange
</commit_message>
<xml_diff>
--- a/data/PC1_PC2_y1_y2_state_interpret_20230323.xlsx
+++ b/data/PC1_PC2_y1_y2_state_interpret_20230323.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wendy/Documents/QTL_manuscript/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A30D87-DD20-B34B-9BE7-44A2E218C1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C133C849-88A7-7B4E-B8C1-51E5A51FB3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13380" yWindow="4220" windowWidth="25020" windowHeight="16440" activeTab="2" xr2:uid="{FA08FE24-FF1E-B64A-8D5B-29A3216B6E47}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>Chr01_13504339_16251328</t>
   </si>
@@ -246,14 +246,20 @@
     <t>Combined</t>
   </si>
   <si>
-    <t>R-square</t>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>Variance explained (%)</t>
+  </si>
+  <si>
+    <t># of QTLs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -283,6 +289,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="MyriadPro-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="MyriadPro-Regular"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -304,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -330,6 +347,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,7 +669,7 @@
       <selection activeCell="C12" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -659,7 +678,7 @@
     <col min="5" max="5" width="101.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -676,7 +695,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -690,7 +709,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>14</v>
@@ -700,7 +719,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -710,7 +729,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>15</v>
@@ -720,7 +739,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="17">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -737,7 +756,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="17">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -754,7 +773,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
@@ -769,7 +788,7 @@
       </c>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" s="7"/>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -780,7 +799,7 @@
       <c r="D9" s="7"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>17</v>
@@ -791,7 +810,7 @@
       <c r="D10" s="7"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>1</v>
@@ -802,7 +821,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>5</v>
       </c>
@@ -819,7 +838,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>18</v>
@@ -830,7 +849,7 @@
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="17">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -847,7 +866,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="34">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -864,10 +883,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:4">
       <c r="D17" s="4"/>
     </row>
   </sheetData>
@@ -894,13 +913,13 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -914,7 +933,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -928,7 +947,7 @@
         <v>3.9319630000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
@@ -942,7 +961,7 @@
         <v>3.9921720000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -956,7 +975,7 @@
         <v>3.9693559999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -970,7 +989,7 @@
         <v>3.958078</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
@@ -984,7 +1003,7 @@
         <v>3.873799</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1006,42 +1025,75 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE2A8AB6-262F-3E43-BF1A-E2E6C4B6E24B}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9">
+        <v>2.34</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" s="9">
+        <v>13.88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>52</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" s="9">
+        <v>15.19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2">
-        <v>2.34</v>
-      </c>
-      <c r="C2">
-        <v>13.88</v>
-      </c>
-      <c r="D2">
-        <v>15.19</v>
-      </c>
-      <c r="E2">
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5" s="9">
         <v>88.22</v>
       </c>
     </row>

</xml_diff>